<commit_message>
wszytsko przygotowane pod capacitor
</commit_message>
<xml_diff>
--- a/database/pasty.xlsx
+++ b/database/pasty.xlsx
@@ -415,7 +415,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,6 +451,19 @@
       </c>
       <c r="C2" t="n">
         <v>2</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>dvd</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>32</v>
+      </c>
+      <c r="C3" t="n">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
strona i logika kondensatora
</commit_message>
<xml_diff>
--- a/database/pasty.xlsx
+++ b/database/pasty.xlsx
@@ -455,7 +455,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -485,6 +485,16 @@
         <v>2</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>testowa</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>